<commit_message>
Change frontend table description to upper case column names
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/frontend_table_description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/frontend_table_description.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreusche.LIFE.000\Nextcloud\arbeit\Teilprojekte\Interpolar\Datenbankstruktur\Release 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-db2frontend\db2frontend\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E13F92-FE5A-4630-BD60-BC546D08665C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="21240" windowHeight="6690" tabRatio="791"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="frontend_table_description" sheetId="15" r:id="rId1"/>
     <sheet name="Ward_Patients" sheetId="13" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="340">
-  <si>
-    <t>column_name</t>
-  </si>
-  <si>
-    <t>resource</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="342">
   <si>
     <t>pat_id</t>
   </si>
@@ -48,12 +43,6 @@
     <t>pat_vorname</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Beschreibung</t>
-  </si>
-  <si>
     <t>record_id</t>
   </si>
   <si>
@@ -1045,12 +1034,30 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>COLUMN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>COLUMN_TYPE</t>
+  </si>
+  <si>
+    <t>TABLE_NAME</t>
+  </si>
+  <si>
+    <t>VALUE_LENGTH</t>
+  </si>
+  <si>
+    <t>VALUE_COUNT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1896,12 +1903,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D476"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F476"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1909,2541 +1914,2534 @@
     <col min="2" max="2" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="136.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="2"/>
+    <col min="5" max="5" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="475" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4455,7 +4453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4466,17 +4464,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>